<commit_message>
More refactoring. BEST VERSION SO FAR. Need to integrate normal, non-parallelizable code
</commit_message>
<xml_diff>
--- a/evograph/analysis/parallelism.xlsx
+++ b/evograph/analysis/parallelism.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="-28800" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,20 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>kValue</t>
+  </si>
+  <si>
+    <t>Threads</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -336,12 +350,91 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="D6:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="6" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="8" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="E8">
+        <f>2*E7</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="E9">
+        <f t="shared" ref="E9:E17" si="0">2*E8</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="15" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="16" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>512</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Cannot remember if i committed
</commit_message>
<xml_diff>
--- a/evograph/analysis/parallelism.xlsx
+++ b/evograph/analysis/parallelism.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-10000" yWindow="460" windowWidth="10000" windowHeight="11340" tabRatio="500"/>
+    <workbookView xWindow="-9980" yWindow="460" windowWidth="10000" windowHeight="11340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>kValue</t>
   </si>
@@ -45,6 +45,24 @@
   </si>
   <si>
     <t>toy.txt</t>
+  </si>
+  <si>
+    <t>10:46.228023</t>
+  </si>
+  <si>
+    <t>12:33.418205</t>
+  </si>
+  <si>
+    <t>11:32.669576</t>
+  </si>
+  <si>
+    <t>3:29.068530</t>
+  </si>
+  <si>
+    <t>4:51.268454</t>
+  </si>
+  <si>
+    <t>6:22.498166</t>
   </si>
 </sst>
 </file>
@@ -86,7 +104,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -364,15 +382,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C6:I65"/>
+  <dimension ref="C6:I66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+    <sheetView tabSelected="1" topLeftCell="D39" workbookViewId="0">
+      <selection activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="6" max="6" width="17.83203125" style="1" customWidth="1"/>
+    <col min="7" max="8" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="6" spans="3:6" x14ac:dyDescent="0.2">
@@ -738,116 +757,211 @@
       <c r="F46" s="1">
         <v>629.74699999999996</v>
       </c>
-      <c r="G46" s="2">
-        <v>4.6449421296296291E-3</v>
-      </c>
-      <c r="H46" s="2">
-        <v>7.4346412037037029E-3</v>
-      </c>
-      <c r="I46" s="2">
-        <v>9.7866435185185192E-3</v>
-      </c>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
     </row>
     <row r="47" spans="3:9" x14ac:dyDescent="0.2">
       <c r="E47">
         <v>2</v>
       </c>
+      <c r="F47" s="1">
+        <v>697.43860133299995</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I47" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="48" spans="3:9" x14ac:dyDescent="0.2">
       <c r="E48">
         <v>8</v>
       </c>
-    </row>
-    <row r="49" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="F48" s="1">
+        <v>294.27833329999999</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I48" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="49" spans="4:9" x14ac:dyDescent="0.2">
       <c r="E49">
         <v>100</v>
       </c>
-    </row>
-    <row r="50" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="F49" s="1">
+        <v>44.271916300000001</v>
+      </c>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2"/>
+      <c r="I49" s="2"/>
+    </row>
+    <row r="50" spans="4:9" x14ac:dyDescent="0.2">
       <c r="E50">
+        <v>110</v>
+      </c>
+      <c r="F50" s="1">
+        <v>65.442959000000002</v>
+      </c>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
+    </row>
+    <row r="51" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="E51">
         <v>200</v>
       </c>
-    </row>
-    <row r="51" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="E51">
+      <c r="F51" s="1">
+        <v>85.492515999999995</v>
+      </c>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
+      <c r="I51" s="2"/>
+    </row>
+    <row r="52" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="E52">
         <v>250</v>
       </c>
-    </row>
-    <row r="52" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="E52">
+      <c r="F52" s="1">
+        <v>108.505737</v>
+      </c>
+      <c r="G52" s="2"/>
+      <c r="H52" s="2"/>
+      <c r="I52" s="2"/>
+    </row>
+    <row r="53" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="E53">
         <v>300</v>
       </c>
-    </row>
-    <row r="53" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="E53">
+      <c r="F53" s="1">
+        <v>130.461792</v>
+      </c>
+      <c r="G53" s="2"/>
+      <c r="H53" s="2"/>
+      <c r="I53" s="2"/>
+    </row>
+    <row r="54" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="E54">
         <v>400</v>
       </c>
-    </row>
-    <row r="54" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="E54">
+      <c r="F54" s="1">
+        <v>165.581974</v>
+      </c>
+      <c r="G54" s="2"/>
+      <c r="H54" s="2"/>
+      <c r="I54" s="2"/>
+    </row>
+    <row r="55" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="E55">
         <v>1000</v>
       </c>
-    </row>
-    <row r="55" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D55">
+      <c r="G55" s="2"/>
+      <c r="H55" s="2"/>
+      <c r="I55" s="2"/>
+    </row>
+    <row r="56" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D56">
         <v>3</v>
       </c>
-      <c r="E55">
+      <c r="E56">
         <v>2</v>
       </c>
-    </row>
-    <row r="56" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="E56">
+      <c r="G56" s="2"/>
+      <c r="H56" s="2"/>
+      <c r="I56" s="2"/>
+    </row>
+    <row r="57" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="E57">
         <v>8</v>
       </c>
-    </row>
-    <row r="57" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="E57">
+      <c r="G57" s="2"/>
+      <c r="H57" s="2"/>
+      <c r="I57" s="2"/>
+    </row>
+    <row r="58" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="E58">
         <v>100</v>
       </c>
-    </row>
-    <row r="58" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="E58">
+      <c r="G58" s="2"/>
+      <c r="H58" s="2"/>
+      <c r="I58" s="2"/>
+    </row>
+    <row r="59" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="E59">
         <v>200</v>
       </c>
-    </row>
-    <row r="59" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="E59">
+      <c r="G59" s="2"/>
+      <c r="H59" s="2"/>
+      <c r="I59" s="2"/>
+    </row>
+    <row r="60" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="E60">
         <v>250</v>
       </c>
-    </row>
-    <row r="60" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="E60">
+      <c r="G60" s="2"/>
+      <c r="H60" s="2"/>
+      <c r="I60" s="2"/>
+    </row>
+    <row r="61" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="E61">
         <v>300</v>
       </c>
-    </row>
-    <row r="61" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="E61">
+      <c r="G61" s="2"/>
+      <c r="H61" s="2"/>
+      <c r="I61" s="2"/>
+    </row>
+    <row r="62" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="E62">
         <v>400</v>
       </c>
-    </row>
-    <row r="62" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="E62">
+      <c r="G62" s="2"/>
+      <c r="H62" s="2"/>
+      <c r="I62" s="2"/>
+    </row>
+    <row r="63" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="E63">
         <v>1000</v>
       </c>
-    </row>
-    <row r="63" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D63">
+      <c r="G63" s="2"/>
+      <c r="H63" s="2"/>
+      <c r="I63" s="2"/>
+    </row>
+    <row r="64" spans="4:9" x14ac:dyDescent="0.2">
+      <c r="D64">
         <v>128</v>
       </c>
-      <c r="E63">
+      <c r="E64">
         <v>1</v>
       </c>
-    </row>
-    <row r="64" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="E64">
+      <c r="G64" s="2"/>
+      <c r="H64" s="2"/>
+      <c r="I64" s="2"/>
+    </row>
+    <row r="65" spans="5:9" x14ac:dyDescent="0.2">
+      <c r="E65">
         <v>2</v>
       </c>
-    </row>
-    <row r="65" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E65">
+      <c r="G65" s="2"/>
+      <c r="H65" s="2"/>
+      <c r="I65" s="2"/>
+    </row>
+    <row r="66" spans="5:9" x14ac:dyDescent="0.2">
+      <c r="E66">
         <v>110</v>
       </c>
+      <c r="G66" s="2"/>
+      <c r="H66" s="2"/>
+      <c r="I66" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>